<commit_message>
feat: Finalizacia a stabilizacia Bazos Scrapera (timeouty, exportovane_data)
</commit_message>
<xml_diff>
--- a/data/bazos_filtre.xlsx
+++ b/data/bazos_filtre.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -42,9 +42,15 @@
     <t>CenaDo</t>
   </si>
   <si>
+    <t>auto</t>
+  </si>
+  <si>
     <t>TC_01</t>
   </si>
   <si>
+    <t>Skoda Octavia</t>
+  </si>
+  <si>
     <t>Ford Focus</t>
   </si>
   <si>
@@ -54,16 +60,7 @@
     <t>TC_03</t>
   </si>
   <si>
-    <t>TC_04</t>
-  </si>
-  <si>
-    <t>TC_05</t>
-  </si>
-  <si>
-    <t>TC_06</t>
-  </si>
-  <si>
-    <t>auto</t>
+    <t>Dacia Duster</t>
   </si>
 </sst>
 </file>
@@ -325,10 +322,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -358,92 +355,75 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
+      <c r="D2" s="1">
+        <v>84102</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>95801</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>2000</v>
+      </c>
+      <c r="G3">
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
         <v>84102</v>
       </c>
-      <c r="E4" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1">
-        <v>84102</v>
-      </c>
-      <c r="E7" s="1">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G7" s="1">
-        <v>5000</v>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>7000</v>
+      </c>
+      <c r="G4">
+        <v>13000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>